<commit_message>
Changed my part, analysis is now done
</commit_message>
<xml_diff>
--- a/Assignment_3/DataVerzamelen_avg speed.xlsx
+++ b/Assignment_3/DataVerzamelen_avg speed.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hugo\Documents\GitHub\EconomicsOfCyber\Assignment_3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
   <si>
     <t>Country</t>
   </si>
@@ -720,9 +725,6 @@
     <t>ZW</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>NoOfBots</t>
   </si>
   <si>
@@ -730,12 +732,18 @@
   </si>
   <si>
     <t>Average connection speed (Mbps)</t>
+  </si>
+  <si>
+    <t>Piracy rate</t>
+  </si>
+  <si>
+    <t>https://torrentfreak.com/europe-has-the-highest-online-piracy-rates-by-far-160801/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0"/>
   </numFmts>
@@ -1116,7 +1124,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1124,41 +1132,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="11.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="11.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1168,8 +1183,11 @@
       <c r="D3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1180,7 +1198,7 @@
         <v>18395</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1199,7 +1217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1228,7 @@
         <v>12144</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1221,7 +1239,7 @@
         <v>10754</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1258,7 @@
         <v>91939</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1253,8 +1271,11 @@
       <c r="D11">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1262,7 +1283,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1276,7 +1297,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1289,8 +1310,11 @@
       <c r="D14">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>16.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1298,7 +1322,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1309,7 +1333,7 @@
         <v>35686</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1317,7 +1341,7 @@
         <v>16546</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1325,15 +1349,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>16509</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1343,8 +1370,11 @@
       <c r="D20">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>14.17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1352,7 +1382,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1362,8 +1392,11 @@
       <c r="D22">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>27.43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1404,7 @@
         <v>6165</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1379,7 +1412,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1420,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1395,7 +1428,7 @@
         <v>6225</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1403,7 +1436,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1411,7 +1444,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1422,7 +1455,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1430,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1440,8 +1473,11 @@
       <c r="D31">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1449,7 +1485,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1457,7 +1493,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1465,15 +1501,18 @@
         <v>384</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2">
         <v>69353</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1481,7 +1520,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1491,8 +1530,11 @@
       <c r="D37">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>11.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1500,7 +1542,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1508,7 +1550,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1516,7 +1558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1524,7 +1566,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1534,8 +1576,11 @@
       <c r="D42">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1543,7 +1588,7 @@
         <v>14696</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1551,7 +1596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1561,8 +1606,11 @@
       <c r="D45">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1570,7 +1618,7 @@
         <v>5033</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1581,7 +1629,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1592,7 +1640,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1603,7 +1651,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1611,7 +1659,7 @@
         <v>25196</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1619,7 +1667,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1627,7 +1675,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1635,7 +1683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1646,7 +1694,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1656,8 +1704,11 @@
       <c r="D55">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1667,8 +1718,11 @@
       <c r="D56">
         <v>14.1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1676,7 +1730,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1686,8 +1740,11 @@
       <c r="D58">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1695,7 +1752,7 @@
         <v>4731</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1703,15 +1760,18 @@
         <v>19549</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="2">
         <v>114749</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>7.13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1722,7 +1782,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -1733,7 +1793,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1743,8 +1803,11 @@
       <c r="D64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -1754,8 +1817,11 @@
       <c r="D65">
         <v>14.1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>22.19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1763,7 +1829,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -1771,7 +1837,7 @@
         <v>12763</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -1782,7 +1848,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -1790,7 +1856,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -1798,7 +1864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -1806,7 +1872,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -1816,8 +1882,11 @@
       <c r="D72">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>8.49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -1825,7 +1894,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -1836,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -1844,7 +1913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -1852,7 +1921,7 @@
         <v>4316</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -1860,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -1868,7 +1937,7 @@
         <v>6877</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -1876,7 +1945,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -1884,7 +1953,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -1892,7 +1961,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -1900,7 +1969,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -1908,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -1916,7 +1985,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -1926,8 +1995,11 @@
       <c r="D85">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>21.87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -1935,7 +2007,7 @@
         <v>17657</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -1943,7 +2015,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -1951,7 +2023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -1959,7 +2031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -1970,7 +2042,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -1978,7 +2050,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -1988,8 +2060,11 @@
       <c r="D92">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -1997,7 +2072,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -2007,8 +2082,11 @@
       <c r="D94">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>8.3699999999999992</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -2018,8 +2096,11 @@
       <c r="D95">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -2029,8 +2110,11 @@
       <c r="D96">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>19.84</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -2040,8 +2124,11 @@
       <c r="D97">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>15.86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -2049,7 +2136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -2059,8 +2146,11 @@
       <c r="D99">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -2068,7 +2158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -2076,7 +2166,7 @@
         <v>31173</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
@@ -2087,7 +2177,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -2095,7 +2185,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
@@ -2105,8 +2195,11 @@
       <c r="D104">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -2114,7 +2207,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
@@ -2122,7 +2215,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -2130,7 +2223,7 @@
         <v>10165</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -2141,7 +2234,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -2152,7 +2245,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
@@ -2160,7 +2253,7 @@
         <v>11546</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
@@ -2168,7 +2261,7 @@
         <v>9965</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -2176,7 +2269,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -2184,7 +2277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -2192,7 +2285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -2203,7 +2296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -2214,7 +2307,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -2222,7 +2315,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -2230,7 +2323,7 @@
         <v>84856</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -2238,7 +2331,7 @@
         <v>4159</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -2246,7 +2339,7 @@
         <v>10533</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -2254,7 +2347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -2265,7 +2358,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
@@ -2273,7 +2366,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
@@ -2281,7 +2374,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -2291,8 +2384,11 @@
       <c r="D125">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>24.54</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
@@ -2303,7 +2399,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
@@ -2313,8 +2409,11 @@
       <c r="D127">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>46.33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
@@ -2322,7 +2421,7 @@
         <v>14742</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
@@ -2333,7 +2432,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
@@ -2341,7 +2440,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
@@ -2349,7 +2448,7 @@
         <v>9476</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
@@ -2357,7 +2456,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
@@ -2365,7 +2464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
@@ -2373,7 +2472,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
@@ -2381,7 +2480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -2389,7 +2488,7 @@
         <v>28479</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
@@ -2397,7 +2496,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
@@ -2405,7 +2504,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
@@ -2413,7 +2512,7 @@
         <v>5076</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
@@ -2421,7 +2520,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
@@ -2429,7 +2528,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
@@ -2440,7 +2539,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
@@ -2448,7 +2547,7 @@
         <v>5139</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
@@ -2456,7 +2555,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
@@ -2464,7 +2563,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
@@ -2474,8 +2573,11 @@
       <c r="D146">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
@@ -2485,8 +2587,11 @@
       <c r="D147">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
@@ -2494,7 +2599,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
@@ -2505,7 +2610,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
@@ -2513,7 +2618,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
@@ -2521,7 +2626,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
@@ -2529,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
@@ -2540,7 +2645,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
@@ -2548,7 +2653,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
@@ -2558,8 +2663,11 @@
       <c r="D155">
         <v>17</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
@@ -2569,8 +2677,11 @@
       <c r="D156">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>12.52</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
@@ -2578,7 +2689,7 @@
         <v>14544</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -2586,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
@@ -2594,7 +2705,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
@@ -2605,7 +2716,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
@@ -2613,7 +2724,7 @@
         <v>9322</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -2624,7 +2735,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -2635,7 +2746,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
@@ -2643,7 +2754,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
@@ -2651,7 +2762,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
@@ -2661,16 +2772,22 @@
       <c r="D166">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B167" s="2">
         <v>250058</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
@@ -2680,8 +2797,11 @@
       <c r="D168">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168">
+        <v>12.55</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
@@ -2689,7 +2809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
@@ -2697,7 +2817,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
@@ -2705,7 +2825,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
@@ -2718,8 +2838,11 @@
       <c r="D172">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172">
+        <v>16.62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
@@ -2730,7 +2853,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
@@ -2744,7 +2867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
@@ -2758,7 +2881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
@@ -2766,7 +2889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
@@ -2779,8 +2902,11 @@
       <c r="D177">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177">
+        <v>19.07</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
@@ -2790,8 +2916,11 @@
       <c r="C178">
         <v>37755</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178">
+        <v>21.31</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
@@ -2804,8 +2933,11 @@
       <c r="D179">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
@@ -2816,7 +2948,7 @@
         <v>8341</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
@@ -2829,8 +2961,11 @@
       <c r="D181">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
@@ -2841,7 +2976,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
@@ -2852,7 +2987,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
@@ -2863,7 +2998,7 @@
         <v>94297</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
@@ -2876,8 +3011,11 @@
       <c r="D185">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185">
+        <v>18.38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
@@ -2890,8 +3028,11 @@
       <c r="D186">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186">
+        <v>12.34</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
@@ -2905,7 +3046,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
@@ -2919,7 +3060,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
@@ -2930,7 +3071,7 @@
         <v>4289</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
@@ -2941,7 +3082,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
@@ -2952,7 +3093,7 @@
         <v>14870</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
@@ -2960,7 +3101,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
@@ -2971,7 +3112,7 @@
         <v>4137</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
@@ -2982,7 +3123,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
@@ -2990,7 +3131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
@@ -2998,7 +3139,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -3009,7 +3150,7 @@
         <v>26610</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
@@ -3017,7 +3158,7 @@
         <v>8079</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
@@ -3028,7 +3169,7 @@
         <v>3430</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
@@ -3036,7 +3177,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
@@ -3047,7 +3188,7 @@
         <v>10441</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
@@ -3058,7 +3199,7 @@
         <v>4520</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
@@ -3071,8 +3212,11 @@
       <c r="D203">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
@@ -3083,7 +3227,7 @@
         <v>6612</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
@@ -3094,7 +3238,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
@@ -3105,7 +3249,7 @@
         <v>36573</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>206</v>
       </c>
@@ -3116,7 +3260,7 @@
         <v>42388</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>207</v>
       </c>
@@ -3127,7 +3271,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>208</v>
       </c>
@@ -3140,8 +3284,11 @@
       <c r="D209">
         <v>7</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>209</v>
       </c>
@@ -3152,7 +3299,7 @@
         <v>22809</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>210</v>
       </c>
@@ -3165,8 +3312,11 @@
       <c r="D211">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>211</v>
       </c>
@@ -3177,7 +3327,7 @@
         <v>46695</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>212</v>
       </c>
@@ -3187,8 +3337,11 @@
       <c r="C213">
         <v>87198</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>213</v>
       </c>
@@ -3199,7 +3352,7 @@
         <v>25613</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>214</v>
       </c>
@@ -3209,8 +3362,11 @@
       <c r="C215">
         <v>2649893</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
@@ -3223,8 +3379,11 @@
       <c r="D216">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>216</v>
       </c>
@@ -3238,7 +3397,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>217</v>
       </c>
@@ -3249,7 +3408,7 @@
         <v>66797</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>218</v>
       </c>
@@ -3257,7 +3416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>219</v>
       </c>
@@ -3268,7 +3427,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>220</v>
       </c>
@@ -3282,7 +3441,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>221</v>
       </c>
@@ -3290,7 +3449,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>222</v>
       </c>
@@ -3298,7 +3457,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>223</v>
       </c>
@@ -3311,8 +3470,11 @@
       <c r="D224">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
@@ -3323,7 +3485,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
@@ -3331,7 +3493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
@@ -3342,7 +3504,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
@@ -3353,7 +3515,7 @@
         <v>31326</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
@@ -3361,7 +3523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>229</v>
       </c>
@@ -3369,7 +3531,7 @@
         <v>16103</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>230</v>
       </c>
@@ -3383,7 +3545,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>231</v>
       </c>
@@ -3394,7 +3556,7 @@
         <v>20574</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
@@ -3405,13 +3567,9 @@
         <v>14193</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B234" s="2">
-        <v>10538915</v>
-      </c>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="1"/>
+      <c r="B234" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>